<commit_message>
modify file integration test
</commit_message>
<xml_diff>
--- a/WIP/Users/HoangLG/CTC_Integration-Test-Case_v1.0_EN.xlsx
+++ b/WIP/Users/HoangLG/CTC_Integration-Test-Case_v1.0_EN.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -210,7 +210,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="215">
   <si>
     <t>TEST CASE</t>
   </si>
@@ -358,15 +358,6 @@
   </si>
   <si>
     <t>Sub total</t>
-  </si>
-  <si>
-    <t>Test coverage</t>
-  </si>
-  <si>
-    <t>%</t>
-  </si>
-  <si>
-    <t>Test successful coverage</t>
   </si>
   <si>
     <t>Back to Test Report</t>
@@ -944,9 +935,6 @@
     <t>Good owner view "Giao dịch của tôi” involve new bill of lading  after Goods Owner create the new bill of lading</t>
   </si>
   <si>
-    <t>không search được với điều kiện cân nặng thể tích</t>
-  </si>
-  <si>
     <t>Carrier view “Thông tin giao dịch" after bid bill of lading</t>
   </si>
   <si>
@@ -974,6 +962,15 @@
   </si>
   <si>
     <t>Admin can't find bill of lading that have been cancelled in "Tìm hàng chuyển" page by Goods Owner.</t>
+  </si>
+  <si>
+    <t>phải login lại mới thấy được tên tài admin thay đổi trên topbar</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>test these case fail before</t>
   </si>
 </sst>
 </file>
@@ -2755,8 +2752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AMK18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2903,11 +2900,17 @@
     </row>
     <row r="13" spans="1:7" ht="21.75" customHeight="1">
       <c r="A13" s="21"/>
-      <c r="B13" s="22"/>
+      <c r="B13" s="22">
+        <v>42845</v>
+      </c>
       <c r="C13" s="23"/>
       <c r="D13" s="27"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="27"/>
+      <c r="E13" s="24" t="s">
+        <v>213</v>
+      </c>
+      <c r="F13" s="27" t="s">
+        <v>214</v>
+      </c>
       <c r="G13" s="28"/>
     </row>
     <row r="14" spans="1:7" ht="19.5" customHeight="1">
@@ -3200,7 +3203,7 @@
   <dimension ref="A1:AMK16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3363,15 +3366,15 @@
       </c>
       <c r="D11" s="78">
         <f>User_Function!A6</f>
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E11" s="78">
         <f>User_Function!B6</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F11" s="78">
         <f>User_Function!C6</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G11" s="78">
         <f>User_Function!D6</f>
@@ -3379,7 +3382,7 @@
       </c>
       <c r="H11" s="79">
         <f>User_Function!E6</f>
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -3392,15 +3395,15 @@
       </c>
       <c r="D12" s="78">
         <f>Admin_Function!A6</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E12" s="78">
         <f>Admin_Function!B6</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F12" s="78">
         <f>Admin_Function!C6</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="G12" s="78">
         <f>Admin_Function!D6</f>
@@ -3408,7 +3411,7 @@
       </c>
       <c r="H12" s="79">
         <f>Admin_Function!E6</f>
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -3419,15 +3422,15 @@
       </c>
       <c r="D13" s="83">
         <f>SUM(D9:D12)</f>
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="E13" s="83">
         <f>SUM(E9:E12)</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F13" s="83">
         <f>SUM(F9:F12)</f>
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="G13" s="83">
         <f>SUM(G9:G12)</f>
@@ -3435,7 +3438,7 @@
       </c>
       <c r="H13" s="84">
         <f>SUM(H9:H12)</f>
-        <v>50</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -3451,34 +3454,20 @@
     <row r="15" spans="1:8">
       <c r="A15" s="66"/>
       <c r="B15" s="66"/>
-      <c r="C15" s="88" t="s">
-        <v>48</v>
-      </c>
+      <c r="C15" s="88"/>
       <c r="D15" s="66"/>
-      <c r="E15" s="89">
-        <f>(D13+E13)*100/(H13-G13)</f>
-        <v>66</v>
-      </c>
-      <c r="F15" s="66" t="s">
-        <v>49</v>
-      </c>
+      <c r="E15" s="89"/>
+      <c r="F15" s="66"/>
       <c r="G15" s="66"/>
       <c r="H15" s="90"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="66"/>
       <c r="B16" s="66"/>
-      <c r="C16" s="88" t="s">
-        <v>50</v>
-      </c>
+      <c r="C16" s="88"/>
       <c r="D16" s="66"/>
-      <c r="E16" s="89">
-        <f>D13*100/(H13-G13)</f>
-        <v>54</v>
-      </c>
-      <c r="F16" s="66" t="s">
-        <v>49</v>
-      </c>
+      <c r="E16" s="89"/>
+      <c r="F16" s="66"/>
       <c r="G16" s="66"/>
       <c r="H16" s="90"/>
     </row>
@@ -3510,8 +3499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:G6"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3533,7 +3522,7 @@
   <sheetData>
     <row r="1" spans="1:257" ht="13.5" customHeight="1">
       <c r="A1" s="93" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94"/>
@@ -3787,10 +3776,10 @@
     </row>
     <row r="2" spans="1:257" ht="13.5" customHeight="1">
       <c r="A2" s="98" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B2" s="139" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C2" s="139"/>
       <c r="D2" s="139"/>
@@ -4047,10 +4036,10 @@
     </row>
     <row r="3" spans="1:257" ht="13.5" customHeight="1">
       <c r="A3" s="100" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B3" s="139" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C3" s="139"/>
       <c r="D3" s="139"/>
@@ -4307,7 +4296,7 @@
     </row>
     <row r="4" spans="1:257" ht="13.5" customHeight="1">
       <c r="A4" s="98" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B4" s="140" t="s">
         <v>4</v>
@@ -4577,7 +4566,7 @@
         <v>44</v>
       </c>
       <c r="E5" s="141" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F5" s="141"/>
       <c r="G5" s="141"/>
@@ -4586,7 +4575,7 @@
       </c>
       <c r="I5" s="97"/>
       <c r="J5" s="97" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="K5" s="97"/>
       <c r="L5" s="97"/>
@@ -4831,24 +4820,24 @@
     </row>
     <row r="6" spans="1:257" ht="13.5" customHeight="1">
       <c r="A6" s="106">
-        <f>COUNTIF(F12:G216,"Pass")</f>
-        <v>21</v>
+        <f>COUNTIF(F12:F48,"Pass")</f>
+        <v>27</v>
       </c>
       <c r="B6" s="107">
         <f>COUNTIF(F13:G663,"Fail")</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C6" s="107">
         <f>E6-D6-B6-A6</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D6" s="108">
         <f>COUNTIF(F13:G663,"N/A")</f>
         <v>0</v>
       </c>
       <c r="E6" s="142">
-        <f>COUNTA(A13:A218)</f>
-        <v>32</v>
+        <f>COUNTA(A11:A48)</f>
+        <v>27</v>
       </c>
       <c r="F6" s="142"/>
       <c r="G6" s="142"/>
@@ -5863,31 +5852,31 @@
     </row>
     <row r="10" spans="1:257" ht="48.75" customHeight="1">
       <c r="A10" s="113" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="113" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="113" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="113" t="s">
         <v>58</v>
       </c>
-      <c r="B10" s="113" t="s">
+      <c r="E10" s="114" t="s">
         <v>59</v>
       </c>
-      <c r="C10" s="113" t="s">
+      <c r="F10" s="114" t="s">
         <v>60</v>
       </c>
-      <c r="D10" s="113" t="s">
+      <c r="G10" s="114" t="s">
         <v>61</v>
       </c>
-      <c r="E10" s="114" t="s">
+      <c r="H10" s="114" t="s">
         <v>62</v>
       </c>
-      <c r="F10" s="114" t="s">
+      <c r="I10" s="113" t="s">
         <v>63</v>
-      </c>
-      <c r="G10" s="114" t="s">
-        <v>64</v>
-      </c>
-      <c r="H10" s="114" t="s">
-        <v>65</v>
-      </c>
-      <c r="I10" s="113" t="s">
-        <v>66</v>
       </c>
       <c r="J10" s="97"/>
       <c r="K10" s="97"/>
@@ -6134,7 +6123,7 @@
     <row r="11" spans="1:257" ht="19.5" customHeight="1">
       <c r="A11" s="115"/>
       <c r="B11" s="115" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C11" s="116"/>
       <c r="D11" s="116"/>
@@ -6391,13 +6380,13 @@
         <v>[User-1]</v>
       </c>
       <c r="B12" s="118" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C12" s="118" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D12" s="118" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E12" s="118"/>
       <c r="F12" s="118" t="s">
@@ -6653,7 +6642,7 @@
     <row r="13" spans="1:257" ht="21.75" customHeight="1">
       <c r="A13" s="115"/>
       <c r="B13" s="115" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C13" s="116"/>
       <c r="D13" s="116"/>
@@ -6910,13 +6899,13 @@
         <v>[User-2]</v>
       </c>
       <c r="B14" s="118" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C14" s="118" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D14" s="118" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E14" s="118"/>
       <c r="F14" s="118" t="s">
@@ -7175,13 +7164,13 @@
         <v>[User-3]</v>
       </c>
       <c r="B15" s="118" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C15" s="118" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D15" s="118" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E15" s="118"/>
       <c r="F15" s="118" t="s">
@@ -7437,7 +7426,7 @@
     <row r="16" spans="1:257" ht="18.75" customHeight="1">
       <c r="A16" s="115"/>
       <c r="B16" s="115" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C16" s="116"/>
       <c r="D16" s="116"/>
@@ -7694,13 +7683,13 @@
         <v>[User-4]</v>
       </c>
       <c r="B17" s="118" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C17" s="118" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D17" s="118" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E17" s="118"/>
       <c r="F17" s="118" t="s">
@@ -7711,7 +7700,7 @@
         <v>42834</v>
       </c>
       <c r="I17" s="118" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="J17" s="97"/>
       <c r="K17" s="97"/>
@@ -7961,13 +7950,13 @@
         <v>[User-5]</v>
       </c>
       <c r="B18" s="118" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C18" s="118" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D18" s="118" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E18" s="118"/>
       <c r="F18" s="118" t="s">
@@ -8223,7 +8212,7 @@
     <row r="19" spans="1:250" ht="24.75" customHeight="1">
       <c r="A19" s="115"/>
       <c r="B19" s="115" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C19" s="116"/>
       <c r="D19" s="116"/>
@@ -8480,13 +8469,13 @@
         <v>[User-6]</v>
       </c>
       <c r="B20" s="118" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C20" s="118" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D20" s="118" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E20" s="118"/>
       <c r="F20" s="118" t="s">
@@ -8497,7 +8486,7 @@
         <v>42834</v>
       </c>
       <c r="I20" s="118" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="J20" s="97"/>
       <c r="K20" s="97"/>
@@ -8747,13 +8736,13 @@
         <v>[User-7]</v>
       </c>
       <c r="B21" s="118" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C21" s="118" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D21" s="120" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E21" s="118"/>
       <c r="F21" s="118" t="s">
@@ -9009,7 +8998,7 @@
     <row r="22" spans="1:250" ht="24" customHeight="1">
       <c r="A22" s="115"/>
       <c r="B22" s="115" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C22" s="116"/>
       <c r="D22" s="116"/>
@@ -9266,13 +9255,13 @@
         <v>[User-8]</v>
       </c>
       <c r="B23" s="118" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C23" s="118" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D23" s="118" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E23" s="118"/>
       <c r="F23" s="118" t="s">
@@ -9531,13 +9520,13 @@
         <v>[User-9]</v>
       </c>
       <c r="B24" s="118" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C24" s="118" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D24" s="118" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E24" s="118"/>
       <c r="F24" s="118" t="s">
@@ -9793,7 +9782,7 @@
     <row r="25" spans="1:250" ht="27.75" customHeight="1">
       <c r="A25" s="115"/>
       <c r="B25" s="115" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C25" s="116"/>
       <c r="D25" s="116"/>
@@ -10050,13 +10039,13 @@
         <v>[User-10]</v>
       </c>
       <c r="B26" s="118" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C26" s="118" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D26" s="118" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E26" s="118"/>
       <c r="F26" s="118" t="s">
@@ -10315,13 +10304,13 @@
         <v>[User-11]</v>
       </c>
       <c r="B27" s="120" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C27" s="120" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D27" s="120" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E27" s="118"/>
       <c r="F27" s="118" t="s">
@@ -10577,7 +10566,7 @@
     <row r="28" spans="1:250" ht="69" customHeight="1">
       <c r="A28" s="116"/>
       <c r="B28" s="115" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C28" s="116"/>
       <c r="D28" s="116"/>
@@ -10834,16 +10823,18 @@
         <v>[User-12]</v>
       </c>
       <c r="B29" s="118" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C29" s="118" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D29" s="118" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E29" s="118"/>
-      <c r="F29" s="118"/>
+      <c r="F29" s="118" t="s">
+        <v>41</v>
+      </c>
       <c r="G29" s="118"/>
       <c r="H29" s="119"/>
       <c r="I29" s="118"/>
@@ -11095,16 +11086,18 @@
         <v>[User-13]</v>
       </c>
       <c r="B30" s="118" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C30" s="120" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D30" s="120" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E30" s="118"/>
-      <c r="F30" s="118"/>
+      <c r="F30" s="118" t="s">
+        <v>41</v>
+      </c>
       <c r="G30" s="118"/>
       <c r="H30" s="119"/>
       <c r="I30" s="118"/>
@@ -11353,7 +11346,7 @@
     <row r="31" spans="1:250" ht="23.25" customHeight="1">
       <c r="A31" s="115"/>
       <c r="B31" s="115" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C31" s="116"/>
       <c r="D31" s="116"/>
@@ -11610,23 +11603,23 @@
         <v>[User-14]</v>
       </c>
       <c r="B32" s="118" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C32" s="118" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D32" s="118" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E32"/>
       <c r="F32" s="118" t="s">
         <v>41</v>
       </c>
       <c r="G32"/>
-      <c r="H32" s="121">
-        <v>42834</v>
-      </c>
-      <c r="I32"/>
+      <c r="H32" s="119">
+        <v>42837</v>
+      </c>
+      <c r="I32" s="118"/>
       <c r="J32" s="97"/>
       <c r="K32" s="97"/>
       <c r="L32" s="97"/>
@@ -11875,13 +11868,13 @@
         <v>[User-15]</v>
       </c>
       <c r="B33" s="118" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C33" s="118" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D33" s="118" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E33" s="118"/>
       <c r="F33" s="118" t="s">
@@ -11891,7 +11884,7 @@
       <c r="H33" s="119">
         <v>42838</v>
       </c>
-      <c r="I33"/>
+      <c r="I33" s="118"/>
       <c r="J33" s="97"/>
       <c r="K33" s="97"/>
       <c r="L33" s="97"/>
@@ -12140,13 +12133,13 @@
         <v>[User-16]</v>
       </c>
       <c r="B34" s="118" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C34" s="118" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D34" s="118" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E34" s="118"/>
       <c r="F34" s="118" t="s">
@@ -12156,7 +12149,7 @@
       <c r="H34" s="119">
         <v>42838</v>
       </c>
-      <c r="I34"/>
+      <c r="I34" s="118"/>
       <c r="J34" s="97"/>
       <c r="K34" s="97"/>
       <c r="L34" s="97"/>
@@ -12405,13 +12398,13 @@
         <v>[User-17]</v>
       </c>
       <c r="B35" s="118" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C35" s="118" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D35" s="118" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E35" s="118"/>
       <c r="F35" s="118" t="s">
@@ -12421,7 +12414,7 @@
       <c r="H35" s="119">
         <v>42838</v>
       </c>
-      <c r="I35"/>
+      <c r="I35" s="118"/>
       <c r="J35" s="97"/>
       <c r="K35" s="97"/>
       <c r="L35" s="97"/>
@@ -12670,25 +12663,23 @@
         <v>[User-18]</v>
       </c>
       <c r="B36" s="118" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C36" s="118" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D36" s="118" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E36" s="118"/>
       <c r="F36" s="118" t="s">
-        <v>42</v>
-      </c>
-      <c r="G36" s="118" t="s">
-        <v>207</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="G36" s="118"/>
       <c r="H36" s="119">
         <v>42838</v>
       </c>
-      <c r="I36"/>
+      <c r="I36" s="118"/>
       <c r="J36" s="97"/>
       <c r="K36" s="97"/>
       <c r="L36" s="97"/>
@@ -12937,23 +12928,23 @@
         <v>[User-19]</v>
       </c>
       <c r="B37" s="118" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C37" s="118" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D37" s="118" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E37" s="118"/>
       <c r="F37" s="118" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G37" s="118"/>
       <c r="H37" s="119">
         <v>42838</v>
       </c>
-      <c r="I37"/>
+      <c r="I37" s="118"/>
       <c r="J37" s="97"/>
       <c r="K37" s="97"/>
       <c r="L37" s="97"/>
@@ -13202,23 +13193,23 @@
         <v>[User-20]</v>
       </c>
       <c r="B38" s="118" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C38" s="118" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D38" s="118" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E38" s="118"/>
       <c r="F38" s="118" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G38" s="118"/>
       <c r="H38" s="119">
         <v>42838</v>
       </c>
-      <c r="I38"/>
+      <c r="I38" s="118"/>
       <c r="J38" s="97"/>
       <c r="K38" s="97"/>
       <c r="L38" s="97"/>
@@ -13464,7 +13455,7 @@
     <row r="39" spans="1:250" ht="51" customHeight="1">
       <c r="A39" s="122"/>
       <c r="B39" s="122" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C39" s="122"/>
       <c r="D39" s="122"/>
@@ -13472,7 +13463,7 @@
       <c r="F39" s="122"/>
       <c r="G39" s="122"/>
       <c r="H39" s="122"/>
-      <c r="I39" s="122"/>
+      <c r="I39" s="118"/>
       <c r="J39" s="97"/>
       <c r="K39" s="97"/>
       <c r="L39" s="97"/>
@@ -13721,23 +13712,23 @@
         <v>[User-21]</v>
       </c>
       <c r="B40" s="118" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C40" s="118" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D40" s="118" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E40"/>
       <c r="F40" s="118" t="s">
         <v>41</v>
       </c>
       <c r="G40"/>
-      <c r="H40" s="121">
-        <v>42834</v>
-      </c>
-      <c r="I40"/>
+      <c r="H40" s="119">
+        <v>42845</v>
+      </c>
+      <c r="I40" s="118"/>
       <c r="J40" s="97"/>
       <c r="K40" s="97"/>
       <c r="L40" s="97"/>
@@ -13986,18 +13977,20 @@
         <v>[User-22]</v>
       </c>
       <c r="B41" s="118" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C41" s="118" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D41" s="118" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E41" s="118"/>
-      <c r="F41" s="118"/>
+      <c r="F41" s="118" t="s">
+        <v>41</v>
+      </c>
       <c r="G41" s="118"/>
-      <c r="H41" s="118"/>
+      <c r="H41" s="119"/>
       <c r="I41" s="118"/>
       <c r="J41" s="97"/>
       <c r="K41" s="97"/>
@@ -14244,7 +14237,7 @@
     <row r="42" spans="1:250" ht="24" customHeight="1">
       <c r="A42" s="122"/>
       <c r="B42" s="122" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C42" s="122"/>
       <c r="D42" s="122"/>
@@ -14501,13 +14494,13 @@
         <v>[User-23]</v>
       </c>
       <c r="B43" s="118" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C43" s="118" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D43" s="118" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E43" s="118"/>
       <c r="F43" s="118" t="s">
@@ -14764,13 +14757,13 @@
         <v>[User-24]</v>
       </c>
       <c r="B44" s="118" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C44" s="118" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D44" s="118" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="E44" s="118"/>
       <c r="F44" s="118" t="s">
@@ -15027,13 +15020,13 @@
         <v>[User-25]</v>
       </c>
       <c r="B45" s="125" t="s">
+        <v>169</v>
+      </c>
+      <c r="C45" s="125" t="s">
+        <v>171</v>
+      </c>
+      <c r="D45" s="125" t="s">
         <v>172</v>
-      </c>
-      <c r="C45" s="125" t="s">
-        <v>174</v>
-      </c>
-      <c r="D45" s="125" t="s">
-        <v>175</v>
       </c>
       <c r="E45" s="125"/>
       <c r="F45" s="125" t="s">
@@ -15041,7 +15034,7 @@
       </c>
       <c r="G45" s="125"/>
       <c r="H45" s="125"/>
-      <c r="I45" s="125"/>
+      <c r="I45" s="118"/>
       <c r="J45" s="97"/>
       <c r="K45" s="97"/>
       <c r="L45" s="97"/>
@@ -15287,7 +15280,7 @@
     <row r="46" spans="1:250" ht="81.75" customHeight="1">
       <c r="A46" s="122"/>
       <c r="B46" s="122" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C46" s="122"/>
       <c r="D46" s="122"/>
@@ -15295,7 +15288,7 @@
       <c r="F46" s="122"/>
       <c r="G46" s="122"/>
       <c r="H46" s="122"/>
-      <c r="I46" s="122"/>
+      <c r="I46" s="118"/>
       <c r="J46" s="97"/>
       <c r="K46" s="97"/>
       <c r="L46" s="97"/>
@@ -15544,20 +15537,20 @@
         <v>[User-26]</v>
       </c>
       <c r="B47" s="118" t="s">
+        <v>174</v>
+      </c>
+      <c r="C47" s="118" t="s">
+        <v>175</v>
+      </c>
+      <c r="D47" s="118" t="s">
         <v>177</v>
       </c>
-      <c r="C47" s="118" t="s">
-        <v>178</v>
-      </c>
-      <c r="D47" s="118" t="s">
-        <v>180</v>
-      </c>
-      <c r="E47"/>
+      <c r="E47" s="118"/>
       <c r="F47" s="118" t="s">
         <v>41</v>
       </c>
-      <c r="G47"/>
-      <c r="H47" s="121">
+      <c r="G47" s="118"/>
+      <c r="H47" s="119">
         <v>42834</v>
       </c>
       <c r="I47"/>
@@ -15809,20 +15802,20 @@
         <v>[User-27]</v>
       </c>
       <c r="B48" s="118" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C48" s="118" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D48" s="118" t="s">
-        <v>180</v>
-      </c>
-      <c r="E48"/>
+        <v>177</v>
+      </c>
+      <c r="E48" s="118"/>
       <c r="F48" s="118" t="s">
         <v>41</v>
       </c>
-      <c r="G48"/>
-      <c r="H48" s="121">
+      <c r="G48" s="118"/>
+      <c r="H48" s="119">
         <v>42834</v>
       </c>
       <c r="I48"/>
@@ -16071,7 +16064,7 @@
     <row r="49" spans="1:1025" ht="30.75" customHeight="1">
       <c r="A49" s="122"/>
       <c r="B49" s="122" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C49" s="122"/>
       <c r="D49" s="122"/>
@@ -16328,20 +16321,20 @@
         <v>ID-29</v>
       </c>
       <c r="B50" s="118" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C50" s="118" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D50" s="118" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E50" s="118"/>
       <c r="F50" s="118"/>
       <c r="G50" s="118"/>
       <c r="H50" s="118"/>
       <c r="I50" s="118" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="51" spans="1:1025" ht="14.25" customHeight="1">
@@ -16350,20 +16343,20 @@
         <v>ID-30</v>
       </c>
       <c r="B51" s="118" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C51" s="118" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D51" s="118" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E51" s="118"/>
       <c r="F51" s="118"/>
       <c r="G51" s="118"/>
       <c r="H51" s="118"/>
       <c r="I51" s="118" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="52" spans="1:1025" ht="14.25" customHeight="1">
@@ -16372,20 +16365,20 @@
         <v>ID-31</v>
       </c>
       <c r="B52" s="118" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C52" s="118" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D52" s="118" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E52" s="118"/>
       <c r="F52" s="118"/>
       <c r="G52" s="118"/>
       <c r="H52" s="118"/>
       <c r="I52" s="118" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="53" spans="1:1025" ht="14.25" customHeight="1">
@@ -16394,20 +16387,20 @@
         <v>ID-32</v>
       </c>
       <c r="B53" s="118" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C53" s="118" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D53" s="118" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E53" s="118"/>
       <c r="F53" s="118"/>
       <c r="G53" s="118"/>
       <c r="H53" s="118"/>
       <c r="I53" s="118" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="54" spans="1:1025" ht="14.25" customHeight="1">
@@ -16416,20 +16409,20 @@
         <v>ID-33</v>
       </c>
       <c r="B54" s="118" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C54" s="118" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D54" s="118" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E54" s="118"/>
       <c r="F54" s="118"/>
       <c r="G54" s="118"/>
       <c r="H54" s="118"/>
       <c r="I54" s="118" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="55" spans="1:1025" ht="14.25" customHeight="1">
@@ -16438,20 +16431,20 @@
         <v>ID-34</v>
       </c>
       <c r="B55" s="118" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C55" s="118" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D55" s="118" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E55" s="118"/>
       <c r="F55" s="118"/>
       <c r="G55" s="118"/>
       <c r="H55" s="118"/>
       <c r="I55" s="118" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="56" spans="1:1025" ht="14.25" customHeight="1">
@@ -16517,8 +16510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK75"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -16540,7 +16533,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="123" customFormat="1">
       <c r="A1" s="93" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94"/>
@@ -16551,10 +16544,10 @@
     </row>
     <row r="2" spans="1:10" ht="14.25" customHeight="1">
       <c r="A2" s="98" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B2" s="139" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C2" s="139"/>
       <c r="D2" s="139"/>
@@ -16567,10 +16560,10 @@
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1">
       <c r="A3" s="100" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B3" s="139" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C3" s="139"/>
       <c r="D3" s="139"/>
@@ -16583,7 +16576,7 @@
     </row>
     <row r="4" spans="1:10" ht="14.25" customHeight="1">
       <c r="A4" s="98" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B4" s="140" t="s">
         <v>4</v>
@@ -16603,40 +16596,40 @@
         <v>42</v>
       </c>
       <c r="C5" s="103" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D5" s="104" t="s">
         <v>44</v>
       </c>
       <c r="E5" s="141" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F5" s="141"/>
       <c r="G5" s="141"/>
       <c r="J5" s="97" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="106">
         <f>COUNTIF(F11:G243,"Pass")</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B6" s="107">
         <f>COUNTIF(F11:G690,"Fail")</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C6" s="107">
         <f>E6-D6-B6-A6</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D6" s="108">
         <f>COUNTIF(F11:G690,"N/A")</f>
         <v>0</v>
       </c>
       <c r="E6" s="142">
-        <f>COUNTA(A11:A247)*2</f>
-        <v>18</v>
+        <f>COUNTA(A11:A22)</f>
+        <v>9</v>
       </c>
       <c r="F6" s="142"/>
       <c r="G6" s="142"/>
@@ -16666,31 +16659,31 @@
     </row>
     <row r="10" spans="1:10" ht="51.75" customHeight="1">
       <c r="A10" s="113" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="113" t="s">
+        <v>149</v>
+      </c>
+      <c r="C10" s="113" t="s">
+        <v>150</v>
+      </c>
+      <c r="D10" s="113" t="s">
         <v>58</v>
       </c>
-      <c r="B10" s="113" t="s">
+      <c r="E10" s="114" t="s">
+        <v>151</v>
+      </c>
+      <c r="F10" s="114" t="s">
         <v>152</v>
       </c>
-      <c r="C10" s="113" t="s">
+      <c r="G10" s="114" t="s">
         <v>153</v>
       </c>
-      <c r="D10" s="113" t="s">
-        <v>61</v>
-      </c>
-      <c r="E10" s="114" t="s">
+      <c r="H10" s="114" t="s">
         <v>154</v>
       </c>
-      <c r="F10" s="114" t="s">
-        <v>155</v>
-      </c>
-      <c r="G10" s="114" t="s">
-        <v>156</v>
-      </c>
-      <c r="H10" s="114" t="s">
-        <v>157</v>
-      </c>
       <c r="I10" s="113" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="87" customHeight="1">
@@ -16699,13 +16692,13 @@
         <v>[Admin-1]</v>
       </c>
       <c r="B11" s="118" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C11" s="118" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D11" s="118" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E11" s="118"/>
       <c r="F11" s="118" t="s">
@@ -16715,7 +16708,9 @@
       <c r="H11" s="119">
         <v>42838</v>
       </c>
-      <c r="I11" s="118"/>
+      <c r="I11" s="118" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="12" spans="1:10" s="124" customFormat="1" ht="78" customHeight="1">
       <c r="A12" s="118" t="str">
@@ -16723,17 +16718,17 @@
         <v>[Admin-2]</v>
       </c>
       <c r="B12" s="118" t="s">
+        <v>181</v>
+      </c>
+      <c r="C12" s="118" t="s">
+        <v>164</v>
+      </c>
+      <c r="D12" s="118" t="s">
         <v>184</v>
-      </c>
-      <c r="C12" s="118" t="s">
-        <v>167</v>
-      </c>
-      <c r="D12" s="118" t="s">
-        <v>187</v>
       </c>
       <c r="E12" s="118"/>
       <c r="F12" s="118" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G12" s="118"/>
       <c r="H12" s="119">
@@ -16747,13 +16742,13 @@
         <v>[Admin-3]</v>
       </c>
       <c r="B13" s="118" t="s">
+        <v>179</v>
+      </c>
+      <c r="C13" s="118" t="s">
         <v>182</v>
       </c>
-      <c r="C13" s="118" t="s">
+      <c r="D13" s="118" t="s">
         <v>185</v>
-      </c>
-      <c r="D13" s="118" t="s">
-        <v>188</v>
       </c>
       <c r="E13" s="118"/>
       <c r="F13" s="118" t="s">
@@ -16771,26 +16766,28 @@
         <v>[Admin-4]</v>
       </c>
       <c r="B14" s="118" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C14" s="118" t="s">
+        <v>183</v>
+      </c>
+      <c r="D14" s="118" t="s">
         <v>186</v>
-      </c>
-      <c r="D14" s="118" t="s">
-        <v>189</v>
       </c>
       <c r="E14" s="118"/>
       <c r="F14" s="118" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G14" s="118"/>
-      <c r="H14" s="119"/>
+      <c r="H14" s="119">
+        <v>42845</v>
+      </c>
       <c r="I14" s="118"/>
     </row>
     <row r="15" spans="1:10" ht="50.25" customHeight="1">
       <c r="A15" s="115"/>
       <c r="B15" s="115" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C15" s="116"/>
       <c r="D15" s="116"/>
@@ -16806,13 +16803,13 @@
         <v>[Admin-5]</v>
       </c>
       <c r="B16" s="118" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C16" s="118" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D16" s="118" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E16"/>
       <c r="F16" s="118" t="s">
@@ -16830,13 +16827,13 @@
         <v>[Admin-6]</v>
       </c>
       <c r="B17" s="118" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C17" s="118" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D17" s="118" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E17" s="118"/>
       <c r="F17" s="118" t="s">
@@ -16851,7 +16848,7 @@
     <row r="18" spans="1:1025" ht="69" customHeight="1">
       <c r="A18" s="122"/>
       <c r="B18" s="122" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C18" s="122"/>
       <c r="D18" s="122"/>
@@ -16867,13 +16864,13 @@
         <v>[Admin-7]</v>
       </c>
       <c r="B19" s="118" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C19" s="118" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D19" s="118" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E19" s="118"/>
       <c r="F19" s="118" t="s">
@@ -16891,13 +16888,13 @@
         <v>[Admin-8]</v>
       </c>
       <c r="B20" s="118" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C20" s="118" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D20" s="118" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E20" s="118"/>
       <c r="F20" s="118" t="s">
@@ -16912,7 +16909,7 @@
     <row r="21" spans="1:1025" ht="43.5" customHeight="1">
       <c r="A21" s="122"/>
       <c r="B21" s="122" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C21" s="122"/>
       <c r="D21" s="122"/>
@@ -16924,27 +16921,27 @@
     </row>
     <row r="22" spans="1:1025" ht="53.25" customHeight="1">
       <c r="A22" s="118" t="str">
-        <f>IF(OR(B22&lt;&gt;"",D22&lt;&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-10,"##")&amp;"]","")</f>
-        <v>[Admin-12]</v>
+        <f>IF(OR(B22&lt;&gt;"",D22&lt;&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-13,"##")&amp;"]","")</f>
+        <v>[Admin-9]</v>
       </c>
       <c r="B22" s="118" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C22" s="118" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D22" s="118" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E22" s="118"/>
       <c r="F22" s="118" t="s">
         <v>41</v>
       </c>
-      <c r="G22"/>
-      <c r="H22" s="121">
+      <c r="G22" s="118"/>
+      <c r="H22" s="119">
         <v>42834</v>
       </c>
-      <c r="I22"/>
+      <c r="I22" s="119"/>
     </row>
     <row r="23" spans="1:1025" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:1025" ht="14.25" customHeight="1"/>

</xml_diff>